<commit_message>
programm read excel data
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1B13919-13E6-4F3B-AD56-E243E1CCC00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darty\Desktop\PycharmProjects\SafeHoles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4B4DFF-B3CF-4C55-8BF9-0C969590AE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Diametro del foro (mm)</t>
   </si>
@@ -42,12 +47,18 @@
   <si>
     <t>F</t>
   </si>
+  <si>
+    <t>choucroute</t>
+  </si>
+  <si>
+    <t>purée</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,15 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -142,6 +147,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -160,7 +172,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -459,334 +471,344 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="9">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
+        <v>600</v>
+      </c>
+      <c r="C3" s="5">
+        <v>50</v>
+      </c>
+      <c r="D3" s="4">
+        <v>550</v>
+      </c>
+      <c r="E3" s="5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
-        <v>4</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7">
-        <v>2</v>
-      </c>
-      <c r="D4" s="6">
-        <v>3</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="B4" s="4">
+        <v>650</v>
+      </c>
+      <c r="C4" s="5">
+        <v>75</v>
+      </c>
+      <c r="D4" s="4">
+        <v>600</v>
+      </c>
+      <c r="E4" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>700</v>
+      </c>
+      <c r="C5" s="5">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4">
+        <v>650</v>
+      </c>
+      <c r="E5" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="9">
+      <c r="B6" s="11">
+        <v>800</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6">
-        <v>8</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="9"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="9"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="9"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="9"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="9"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="9"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="9"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="9"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="9"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="9"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="9"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="9"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="9"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="9"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="9"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="9"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="9"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="9"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="9"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="9"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="9"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="9"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="9"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="9"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="9"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="9"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="9"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="9"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="9"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="9"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="9"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="B40" s="6"/>
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="B42" s="6"/>
-      <c r="C42" s="7"/>
+      <c r="E6" s="5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>